<commit_message>
data analasys code to run on exp machine
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset.xlsx
+++ b/dataAnalysisCodes/watchERP/01-preprocess-plot/watchErpDataset.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="69">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>session directory</t>
-  </si>
-  <si>
-    <t>file name</t>
-  </si>
-  <si>
     <t>condition</t>
   </si>
   <si>
@@ -36,9 +30,6 @@
     <t>2013-01-17-Adrien</t>
   </si>
   <si>
-    <t xml:space="preserve">Adrien </t>
-  </si>
-  <si>
     <t>17/01/2013</t>
   </si>
   <si>
@@ -102,12 +93,6 @@
     <t>ssvep-15Hz</t>
   </si>
   <si>
-    <t>subject name</t>
-  </si>
-  <si>
-    <t>subject tag</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -166,6 +151,78 @@
   </si>
   <si>
     <t>2013-01-18-16-47-38</t>
+  </si>
+  <si>
+    <t>Adrien</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>Marijn</t>
+  </si>
+  <si>
+    <t>24/01/2013</t>
+  </si>
+  <si>
+    <t>2013-01-24-Marijn</t>
+  </si>
+  <si>
+    <t>2013-01-24-15-51-15</t>
+  </si>
+  <si>
+    <t>2013-01-24-15-59-51</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-15-23</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-23-06</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-29-32</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-36-07</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-41-47</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-47-44</t>
+  </si>
+  <si>
+    <t>2013-01-24-16-55-12</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-02-47</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-09-32</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-22-32</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-28-53</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-34-15</t>
+  </si>
+  <si>
+    <t>2013-01-24-17-39-42</t>
+  </si>
+  <si>
+    <t>subjectName</t>
+  </si>
+  <si>
+    <t>sessionDirectory</t>
+  </si>
+  <si>
+    <t>fileName</t>
+  </si>
+  <si>
+    <t>subjectTag</t>
   </si>
 </sst>
 </file>
@@ -518,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,45 +595,45 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -584,22 +641,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -607,22 +664,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
@@ -630,22 +687,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2">
         <v>2</v>
@@ -653,22 +710,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2">
         <v>2</v>
@@ -676,22 +733,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2">
         <v>2</v>
@@ -699,22 +756,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2">
         <v>1</v>
@@ -722,22 +779,22 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
@@ -745,22 +802,22 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2">
         <v>1</v>
@@ -768,22 +825,22 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G11" s="2">
         <v>2</v>
@@ -791,22 +848,22 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2">
         <v>3</v>
@@ -814,22 +871,22 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G13" s="2">
         <v>3</v>
@@ -837,22 +894,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G14" s="2">
         <v>3</v>
@@ -860,22 +917,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G15" s="2">
         <v>3</v>
@@ -883,22 +940,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" s="2">
         <v>3</v>
@@ -906,22 +963,22 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
@@ -929,22 +986,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F18" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G18" s="2">
         <v>1</v>
@@ -952,22 +1009,22 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G19" s="2">
         <v>1</v>
@@ -975,22 +1032,22 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
@@ -998,22 +1055,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G21" s="2">
         <v>2</v>
@@ -1021,22 +1078,22 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G22" s="2">
         <v>1</v>
@@ -1044,22 +1101,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
@@ -1067,22 +1124,22 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G24" s="2">
         <v>2</v>
@@ -1090,22 +1147,22 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G25" s="2">
         <v>3</v>
@@ -1113,22 +1170,22 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G26" s="2">
         <v>2</v>
@@ -1136,22 +1193,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G27" s="2">
         <v>3</v>
@@ -1159,22 +1216,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G28" s="2">
         <v>3</v>
@@ -1182,22 +1239,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G29" s="2">
         <v>2</v>
@@ -1205,22 +1262,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2">
         <v>3</v>
@@ -1228,24 +1285,369 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G31" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="2">
+      <c r="E32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G45" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G46" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>